<commit_message>
ECS-9 added EvaluationResultsHistoryBean#classifierOptions field for xls report
</commit_message>
<xml_diff>
--- a/eca-ers/src/main/resources/report-templates/evaluation-results-history-report-template.xlsx
+++ b/eca-ers/src/main/resources/report-templates/evaluation-results-history-report-template.xlsx
@@ -38,7 +38,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:area(lastCell="I10")</t>
+          <t>jx:area(lastCell="J10")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:if(condition="not empty(report.searchQuery)", lastCell="I3", areas=["A3:B3"])</t>
+          <t>jx:if(condition="not empty(report.searchQuery)", lastCell="J3", areas=["A3:B3"])</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.filters" var="filter" lastCell="I6"</t>
+          <t>jx:each(items="report.filters" var="filter" lastCell="J6"</t>
         </r>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>", lastCell="I4", areas=["A4:B4"])</t>
+          <t>", lastCell="J4", areas=["A4:B4"])</t>
         </r>
       </text>
     </comment>
@@ -138,7 +138,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>", lastCell="I5", areas=["A5:B5"])</t>
+          <t>", lastCell="J5", areas=["A5:B5"])</t>
         </r>
       </text>
     </comment>
@@ -169,7 +169,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>", lastCell="I6", areas=["A6:B6"])</t>
+          <t>", lastCell="J6", areas=["A6:B6"])</t>
         </r>
       </text>
     </comment>
@@ -194,7 +194,7 @@
             <color rgb="000000" tint="0"/>
             <sz val="9"/>
           </rPr>
-          <t>jx:each(items="report.items" var="item" lastCell="I9")</t>
+          <t>jx:each(items="report.items" var="item" lastCell="J9")</t>
         </r>
       </text>
     </comment>
@@ -288,6 +288,9 @@
     <t>Метод оценки точности</t>
   </si>
   <si>
+    <t>Настройки классификатора</t>
+  </si>
+  <si>
     <t>Точность классификатора, %</t>
   </si>
   <si>
@@ -329,6 +332,16 @@
   </si>
   <si>
     <t>${item.evaluationMethod}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="000000" tint="0"/>
+        <sz val="11"/>
+      </rPr>
+      <t>${item.classifierOptions}</t>
+    </r>
   </si>
   <si>
     <r>
@@ -742,7 +755,7 @@
   <sheetPr>
     <outlinePr summaryBelow="true" summaryRight="true"/>
   </sheetPr>
-  <dimension ref="A1:AMK10"/>
+  <dimension ref="A1:AML10"/>
   <sheetViews>
     <sheetView showZeros="true" workbookViewId="0"/>
   </sheetViews>
@@ -750,18 +763,18 @@
   <cols>
     <col customWidth="true" max="1" min="1" outlineLevel="0" width="43.6640623533012"/>
     <col customWidth="true" max="2" min="2" outlineLevel="0" width="40.2187508193987"/>
-    <col customWidth="true" max="4" min="3" outlineLevel="0" width="38.664062184135"/>
-    <col customWidth="true" hidden="false" max="5" min="5" outlineLevel="0" width="37.7070606750035"/>
-    <col customWidth="true" hidden="false" max="6" min="6" outlineLevel="0" width="28.8425687072676"/>
-    <col customWidth="true" max="7" min="7" outlineLevel="0" width="32.3320312612337"/>
-    <col customWidth="true" max="8" min="8" outlineLevel="0" width="51.8867161748414"/>
-    <col customWidth="true" max="9" min="9" outlineLevel="0" width="57.7773424568038"/>
-    <col customWidth="true" max="10" min="10" outlineLevel="0" width="26.9999998308338"/>
-    <col customWidth="true" max="11" min="11" outlineLevel="0" width="30.8867187123341"/>
-    <col customWidth="true" max="12" min="12" outlineLevel="0" width="34.3320302462366"/>
-    <col customWidth="true" max="13" min="13" outlineLevel="0" width="31.4414051484374"/>
-    <col customWidth="true" max="14" min="14" outlineLevel="0" width="31.5546869436019"/>
-    <col customWidth="true" max="1025" min="15" outlineLevel="0" width="8.55468778943276"/>
+    <col customWidth="true" max="5" min="3" outlineLevel="0" width="38.664062184135"/>
+    <col customWidth="true" hidden="false" max="6" min="6" outlineLevel="0" width="37.7070606750035"/>
+    <col customWidth="true" hidden="false" max="7" min="7" outlineLevel="0" width="28.8425687072676"/>
+    <col customWidth="true" max="8" min="8" outlineLevel="0" width="32.3320312612337"/>
+    <col customWidth="true" max="9" min="9" outlineLevel="0" width="51.8867161748414"/>
+    <col customWidth="true" max="10" min="10" outlineLevel="0" width="57.7773424568038"/>
+    <col customWidth="true" max="11" min="11" outlineLevel="0" width="26.9999998308338"/>
+    <col customWidth="true" max="12" min="12" outlineLevel="0" width="30.8867187123341"/>
+    <col customWidth="true" max="13" min="13" outlineLevel="0" width="34.3320302462366"/>
+    <col customWidth="true" max="14" min="14" outlineLevel="0" width="31.4414051484374"/>
+    <col customWidth="true" max="15" min="15" outlineLevel="0" width="31.5546869436019"/>
+    <col customWidth="true" max="1026" min="16" outlineLevel="0" width="8.55468778943276"/>
   </cols>
   <sheetData>
     <row ht="15.6000003814697" outlineLevel="0" r="1">
@@ -776,11 +789,12 @@
       <c r="G1" s="1" t="s"/>
       <c r="H1" s="1" t="s"/>
       <c r="I1" s="1" t="s"/>
-      <c r="J1" s="0" t="n"/>
+      <c r="J1" s="1" t="s"/>
       <c r="K1" s="0" t="n"/>
       <c r="L1" s="0" t="n"/>
       <c r="M1" s="0" t="n"/>
       <c r="N1" s="0" t="n"/>
+      <c r="O1" s="0" t="n"/>
     </row>
     <row ht="15.6000003814697" outlineLevel="0" r="2">
       <c r="A2" s="2" t="n"/>
@@ -792,11 +806,12 @@
       <c r="G2" s="3" t="n"/>
       <c r="H2" s="3" t="n"/>
       <c r="I2" s="3" t="n"/>
-      <c r="J2" s="0" t="n"/>
+      <c r="J2" s="3" t="n"/>
       <c r="K2" s="0" t="n"/>
       <c r="L2" s="0" t="n"/>
       <c r="M2" s="0" t="n"/>
       <c r="N2" s="0" t="n"/>
+      <c r="O2" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="3">
       <c r="A3" s="4" t="s">
@@ -812,11 +827,12 @@
       <c r="G3" s="5" t="s"/>
       <c r="H3" s="5" t="s"/>
       <c r="I3" s="5" t="s"/>
-      <c r="J3" s="0" t="n"/>
+      <c r="J3" s="5" t="s"/>
       <c r="K3" s="0" t="n"/>
       <c r="L3" s="0" t="n"/>
       <c r="M3" s="0" t="n"/>
       <c r="N3" s="0" t="n"/>
+      <c r="O3" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="4">
       <c r="A4" s="6" t="s">
@@ -832,11 +848,12 @@
       <c r="G4" s="7" t="s"/>
       <c r="H4" s="7" t="s"/>
       <c r="I4" s="7" t="s"/>
-      <c r="J4" s="0" t="n"/>
+      <c r="J4" s="7" t="s"/>
       <c r="K4" s="0" t="n"/>
       <c r="L4" s="0" t="n"/>
       <c r="M4" s="0" t="n"/>
       <c r="N4" s="0" t="n"/>
+      <c r="O4" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="5">
       <c r="A5" s="6" t="s">
@@ -852,11 +869,12 @@
       <c r="G5" s="7" t="s"/>
       <c r="H5" s="7" t="s"/>
       <c r="I5" s="7" t="s"/>
-      <c r="J5" s="0" t="n"/>
+      <c r="J5" s="7" t="s"/>
       <c r="K5" s="0" t="n"/>
       <c r="L5" s="0" t="n"/>
       <c r="M5" s="0" t="n"/>
       <c r="N5" s="0" t="n"/>
+      <c r="O5" s="0" t="n"/>
     </row>
     <row customHeight="true" ht="14.8500003814697" outlineLevel="0" r="6">
       <c r="A6" s="6" t="s">
@@ -872,11 +890,12 @@
       <c r="G6" s="7" t="s"/>
       <c r="H6" s="7" t="s"/>
       <c r="I6" s="7" t="s"/>
-      <c r="J6" s="0" t="n"/>
+      <c r="J6" s="7" t="s"/>
       <c r="K6" s="0" t="n"/>
       <c r="L6" s="0" t="n"/>
       <c r="M6" s="0" t="n"/>
       <c r="N6" s="0" t="n"/>
+      <c r="O6" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="3" t="n"/>
@@ -888,11 +907,12 @@
       <c r="G7" s="3" t="n"/>
       <c r="H7" s="3" t="n"/>
       <c r="I7" s="3" t="n"/>
-      <c r="J7" s="0" t="n"/>
+      <c r="J7" s="3" t="n"/>
       <c r="K7" s="0" t="n"/>
       <c r="L7" s="0" t="n"/>
       <c r="M7" s="0" t="n"/>
       <c r="N7" s="0" t="n"/>
+      <c r="O7" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="8" t="s">
@@ -916,55 +936,61 @@
       <c r="G8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="10" t="n"/>
+      <c r="J8" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="K8" s="10" t="n"/>
       <c r="L8" s="10" t="n"/>
       <c r="M8" s="10" t="n"/>
       <c r="N8" s="10" t="n"/>
+      <c r="O8" s="10" t="n"/>
     </row>
     <row customHeight="true" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="0" t="n"/>
+      <c r="I9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="K9" s="0" t="n"/>
       <c r="L9" s="0" t="n"/>
       <c r="M9" s="0" t="n"/>
       <c r="N9" s="0" t="n"/>
+      <c r="O9" s="0" t="n"/>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="15" t="s"/>
       <c r="C10" s="15" t="s"/>
@@ -973,21 +999,22 @@
       <c r="F10" s="15" t="s"/>
       <c r="G10" s="15" t="s"/>
       <c r="H10" s="15" t="s"/>
-      <c r="I10" s="16" t="s"/>
-      <c r="J10" s="0" t="n"/>
+      <c r="I10" s="15" t="s"/>
+      <c r="J10" s="16" t="s"/>
       <c r="K10" s="0" t="n"/>
       <c r="L10" s="0" t="n"/>
       <c r="M10" s="0" t="n"/>
       <c r="N10" s="0" t="n"/>
+      <c r="O10" s="0" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A10:J10"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.511805534362793" header="0.511805534362793" left="0.700000047683716" right="0.700000047683716" top="0.75"/>
   <pageSetup fitToHeight="0" fitToWidth="0" orientation="portrait" paperHeight="297mm" paperSize="9" paperWidth="210mm" scale="100"/>

</xml_diff>